<commit_message>
Refactor battle mechanics and GUI; enhance Pokémon selection and battle logic
</commit_message>
<xml_diff>
--- a/datos/pokemon_primera_gen.xlsx
+++ b/datos/pokemon_primera_gen.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G152"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Movimiento 3</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Movimiento 4</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Sprite URL</t>
         </is>
       </c>
@@ -489,15 +499,25 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/1.png</t>
         </is>
@@ -522,15 +542,25 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/2.png</t>
         </is>
@@ -555,15 +585,25 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/3.png</t>
         </is>
@@ -588,15 +628,25 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/4.png</t>
         </is>
@@ -621,15 +671,25 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/5.png</t>
         </is>
@@ -654,15 +714,25 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/6.png</t>
         </is>
@@ -687,15 +757,25 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/7.png</t>
         </is>
@@ -720,15 +800,25 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/8.png</t>
         </is>
@@ -753,15 +843,25 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/9.png</t>
         </is>
@@ -786,15 +886,25 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/10.png</t>
         </is>
@@ -819,15 +929,25 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/11.png</t>
         </is>
@@ -852,15 +972,25 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/12.png</t>
         </is>
@@ -885,15 +1015,25 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/13.png</t>
         </is>
@@ -918,15 +1058,25 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/14.png</t>
         </is>
@@ -951,15 +1101,25 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/15.png</t>
         </is>
@@ -989,10 +1149,20 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/16.png</t>
         </is>
@@ -1022,10 +1192,20 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/17.png</t>
         </is>
@@ -1055,10 +1235,20 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/18.png</t>
         </is>
@@ -1088,10 +1278,20 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/19.png</t>
         </is>
@@ -1121,10 +1321,20 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/20.png</t>
         </is>
@@ -1154,10 +1364,20 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/21.png</t>
         </is>
@@ -1187,10 +1407,20 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/22.png</t>
         </is>
@@ -1215,15 +1445,25 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/23.png</t>
         </is>
@@ -1248,15 +1488,25 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/24.png</t>
         </is>
@@ -1281,15 +1531,25 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/25.png</t>
         </is>
@@ -1314,15 +1574,25 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/26.png</t>
         </is>
@@ -1347,15 +1617,25 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/27.png</t>
         </is>
@@ -1380,15 +1660,25 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/28.png</t>
         </is>
@@ -1413,15 +1703,25 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/29.png</t>
         </is>
@@ -1446,15 +1746,25 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/30.png</t>
         </is>
@@ -1479,15 +1789,25 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/31.png</t>
         </is>
@@ -1512,15 +1832,25 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/32.png</t>
         </is>
@@ -1545,15 +1875,25 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/33.png</t>
         </is>
@@ -1578,15 +1918,25 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/34.png</t>
         </is>
@@ -1611,15 +1961,25 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Tackle (fairy, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Quick Attack (fairy, 50)</t>
+          <t>Fairy Move (fairy, 60)</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Fairy Blast (fairy, 80)</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/35.png</t>
         </is>
@@ -1644,15 +2004,25 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Tackle (fairy, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Quick Attack (fairy, 50)</t>
+          <t>Fairy Move (fairy, 60)</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Fairy Blast (fairy, 80)</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/36.png</t>
         </is>
@@ -1677,15 +2047,25 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/37.png</t>
         </is>
@@ -1710,15 +2090,25 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/38.png</t>
         </is>
@@ -1748,10 +2138,20 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/39.png</t>
         </is>
@@ -1781,10 +2181,20 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/40.png</t>
         </is>
@@ -1809,15 +2219,25 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/41.png</t>
         </is>
@@ -1842,15 +2262,25 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/42.png</t>
         </is>
@@ -1875,15 +2305,25 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/43.png</t>
         </is>
@@ -1908,15 +2348,25 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/44.png</t>
         </is>
@@ -1941,15 +2391,25 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/45.png</t>
         </is>
@@ -1974,15 +2434,25 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/46.png</t>
         </is>
@@ -2007,15 +2477,25 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/47.png</t>
         </is>
@@ -2040,15 +2520,25 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/48.png</t>
         </is>
@@ -2073,15 +2563,25 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/49.png</t>
         </is>
@@ -2106,15 +2606,25 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/50.png</t>
         </is>
@@ -2139,15 +2649,25 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/51.png</t>
         </is>
@@ -2177,10 +2697,20 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/52.png</t>
         </is>
@@ -2210,10 +2740,20 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/53.png</t>
         </is>
@@ -2238,15 +2778,25 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/54.png</t>
         </is>
@@ -2271,15 +2821,25 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/55.png</t>
         </is>
@@ -2304,15 +2864,25 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Tackle (fighting, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Quick Attack (fighting, 50)</t>
+          <t>Fighting Move (fighting, 60)</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Fighting Blast (fighting, 80)</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/56.png</t>
         </is>
@@ -2337,15 +2907,25 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Tackle (fighting, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Quick Attack (fighting, 50)</t>
+          <t>Fighting Move (fighting, 60)</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Fighting Blast (fighting, 80)</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/57.png</t>
         </is>
@@ -2370,15 +2950,25 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/58.png</t>
         </is>
@@ -2403,15 +2993,25 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/59.png</t>
         </is>
@@ -2436,15 +3036,25 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/60.png</t>
         </is>
@@ -2469,15 +3079,25 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/61.png</t>
         </is>
@@ -2502,15 +3122,25 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/62.png</t>
         </is>
@@ -2535,15 +3165,25 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/63.png</t>
         </is>
@@ -2568,15 +3208,25 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/64.png</t>
         </is>
@@ -2601,15 +3251,25 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/65.png</t>
         </is>
@@ -2634,15 +3294,25 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Tackle (fighting, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Quick Attack (fighting, 50)</t>
+          <t>Fighting Move (fighting, 60)</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Fighting Blast (fighting, 80)</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/66.png</t>
         </is>
@@ -2667,15 +3337,25 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Tackle (fighting, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Quick Attack (fighting, 50)</t>
+          <t>Fighting Move (fighting, 60)</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Fighting Blast (fighting, 80)</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/67.png</t>
         </is>
@@ -2700,15 +3380,25 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Tackle (fighting, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Quick Attack (fighting, 50)</t>
+          <t>Fighting Move (fighting, 60)</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Fighting Blast (fighting, 80)</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/68.png</t>
         </is>
@@ -2733,15 +3423,25 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/69.png</t>
         </is>
@@ -2766,15 +3466,25 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/70.png</t>
         </is>
@@ -2799,15 +3509,25 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/71.png</t>
         </is>
@@ -2832,15 +3552,25 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/72.png</t>
         </is>
@@ -2865,15 +3595,25 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/73.png</t>
         </is>
@@ -2898,15 +3638,25 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/74.png</t>
         </is>
@@ -2931,15 +3681,25 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/75.png</t>
         </is>
@@ -2964,15 +3724,25 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/76.png</t>
         </is>
@@ -2997,15 +3767,25 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/77.png</t>
         </is>
@@ -3030,15 +3810,25 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/78.png</t>
         </is>
@@ -3063,15 +3853,25 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/79.png</t>
         </is>
@@ -3096,15 +3896,25 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/80.png</t>
         </is>
@@ -3129,15 +3939,25 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/81.png</t>
         </is>
@@ -3162,15 +3982,25 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/82.png</t>
         </is>
@@ -3200,10 +4030,20 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/83.png</t>
         </is>
@@ -3233,10 +4073,20 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/84.png</t>
         </is>
@@ -3266,10 +4116,20 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/85.png</t>
         </is>
@@ -3294,15 +4154,25 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/86.png</t>
         </is>
@@ -3327,15 +4197,25 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/87.png</t>
         </is>
@@ -3360,15 +4240,25 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/88.png</t>
         </is>
@@ -3393,15 +4283,25 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/89.png</t>
         </is>
@@ -3426,15 +4326,25 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/90.png</t>
         </is>
@@ -3459,15 +4369,25 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/91.png</t>
         </is>
@@ -3492,15 +4412,25 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Tackle (ghost, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Quick Attack (ghost, 50)</t>
+          <t>Ghost Move (ghost, 60)</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Ghost Blast (ghost, 80)</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/92.png</t>
         </is>
@@ -3525,15 +4455,25 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Tackle (ghost, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Quick Attack (ghost, 50)</t>
+          <t>Ghost Move (ghost, 60)</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Ghost Blast (ghost, 80)</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/93.png</t>
         </is>
@@ -3558,15 +4498,25 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Tackle (ghost, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Quick Attack (ghost, 50)</t>
+          <t>Ghost Move (ghost, 60)</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Ghost Blast (ghost, 80)</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/94.png</t>
         </is>
@@ -3591,15 +4541,25 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/95.png</t>
         </is>
@@ -3624,15 +4584,25 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/96.png</t>
         </is>
@@ -3657,15 +4627,25 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/97.png</t>
         </is>
@@ -3690,15 +4670,25 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/98.png</t>
         </is>
@@ -3723,15 +4713,25 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/99.png</t>
         </is>
@@ -3756,15 +4756,25 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/100.png</t>
         </is>
@@ -3789,15 +4799,25 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/101.png</t>
         </is>
@@ -3822,15 +4842,25 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/102.png</t>
         </is>
@@ -3855,15 +4885,25 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/103.png</t>
         </is>
@@ -3888,15 +4928,25 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/104.png</t>
         </is>
@@ -3921,15 +4971,25 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/105.png</t>
         </is>
@@ -3954,15 +5014,25 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Tackle (fighting, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Quick Attack (fighting, 50)</t>
+          <t>Fighting Move (fighting, 60)</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Fighting Blast (fighting, 80)</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/106.png</t>
         </is>
@@ -3987,15 +5057,25 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Tackle (fighting, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Quick Attack (fighting, 50)</t>
+          <t>Fighting Move (fighting, 60)</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Fighting Blast (fighting, 80)</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/107.png</t>
         </is>
@@ -4025,10 +5105,20 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/108.png</t>
         </is>
@@ -4053,15 +5143,25 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/109.png</t>
         </is>
@@ -4086,15 +5186,25 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Tackle (poison, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Quick Attack (poison, 50)</t>
+          <t>Poison Move (poison, 60)</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Poison Blast (poison, 80)</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/110.png</t>
         </is>
@@ -4119,15 +5229,25 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/111.png</t>
         </is>
@@ -4152,15 +5272,25 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Tackle (ground, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Quick Attack (ground, 50)</t>
+          <t>Ground Move (ground, 60)</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Ground Blast (ground, 80)</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/112.png</t>
         </is>
@@ -4190,10 +5320,20 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/113.png</t>
         </is>
@@ -4218,15 +5358,25 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Tackle (grass, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Quick Attack (grass, 50)</t>
+          <t>Grass Move (grass, 60)</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Grass Blast (grass, 80)</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/114.png</t>
         </is>
@@ -4256,10 +5406,20 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/115.png</t>
         </is>
@@ -4284,15 +5444,25 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/116.png</t>
         </is>
@@ -4317,15 +5487,25 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/117.png</t>
         </is>
@@ -4350,15 +5530,25 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/118.png</t>
         </is>
@@ -4383,15 +5573,25 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/119.png</t>
         </is>
@@ -4416,15 +5616,25 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/120.png</t>
         </is>
@@ -4449,15 +5659,25 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/121.png</t>
         </is>
@@ -4482,15 +5702,25 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/122.png</t>
         </is>
@@ -4515,15 +5745,25 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/123.png</t>
         </is>
@@ -4548,15 +5788,25 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Tackle (ice, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Quick Attack (ice, 50)</t>
+          <t>Ice Move (ice, 60)</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Ice Blast (ice, 80)</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/124.png</t>
         </is>
@@ -4581,15 +5831,25 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/125.png</t>
         </is>
@@ -4614,15 +5874,25 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/126.png</t>
         </is>
@@ -4647,15 +5917,25 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Tackle (bug, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Quick Attack (bug, 50)</t>
+          <t>Bug Move (bug, 60)</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Bug Blast (bug, 80)</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/127.png</t>
         </is>
@@ -4685,10 +5965,20 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/128.png</t>
         </is>
@@ -4713,15 +6003,25 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/129.png</t>
         </is>
@@ -4746,15 +6046,25 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/130.png</t>
         </is>
@@ -4779,15 +6089,25 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/131.png</t>
         </is>
@@ -4817,10 +6137,20 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/132.png</t>
         </is>
@@ -4850,10 +6180,20 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/133.png</t>
         </is>
@@ -4878,15 +6218,25 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Tackle (water, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Quick Attack (water, 50)</t>
+          <t>Water Move (water, 60)</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Water Blast (water, 80)</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/134.png</t>
         </is>
@@ -4911,15 +6261,25 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/135.png</t>
         </is>
@@ -4944,15 +6304,25 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/136.png</t>
         </is>
@@ -4982,10 +6352,20 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/137.png</t>
         </is>
@@ -5010,15 +6390,25 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/138.png</t>
         </is>
@@ -5043,15 +6433,25 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/139.png</t>
         </is>
@@ -5076,15 +6476,25 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/140.png</t>
         </is>
@@ -5109,15 +6519,25 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/141.png</t>
         </is>
@@ -5142,15 +6562,25 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Tackle (rock, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>Quick Attack (rock, 50)</t>
+          <t>Rock Move (rock, 60)</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Rock Blast (rock, 80)</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/142.png</t>
         </is>
@@ -5180,10 +6610,20 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>Quick Attack (normal, 50)</t>
+          <t>Normal Move (normal, 60)</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Normal Blast (normal, 80)</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/143.png</t>
         </is>
@@ -5208,15 +6648,25 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Tackle (ice, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>Quick Attack (ice, 50)</t>
+          <t>Ice Move (ice, 60)</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Ice Blast (ice, 80)</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/144.png</t>
         </is>
@@ -5241,15 +6691,25 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Tackle (electric, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>Quick Attack (electric, 50)</t>
+          <t>Electric Move (electric, 60)</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Electric Blast (electric, 80)</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/145.png</t>
         </is>
@@ -5274,15 +6734,25 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Tackle (fire, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>Quick Attack (fire, 50)</t>
+          <t>Fire Move (fire, 60)</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Fire Blast (fire, 80)</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/146.png</t>
         </is>
@@ -5307,15 +6777,25 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Tackle (dragon, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Quick Attack (dragon, 50)</t>
+          <t>Dragon Move (dragon, 60)</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Dragon Blast (dragon, 80)</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/147.png</t>
         </is>
@@ -5340,15 +6820,25 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Tackle (dragon, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Quick Attack (dragon, 50)</t>
+          <t>Dragon Move (dragon, 60)</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Dragon Blast (dragon, 80)</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/148.png</t>
         </is>
@@ -5373,15 +6863,25 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Tackle (dragon, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Quick Attack (dragon, 50)</t>
+          <t>Dragon Move (dragon, 60)</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Dragon Blast (dragon, 80)</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/149.png</t>
         </is>
@@ -5406,15 +6906,25 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/150.png</t>
         </is>
@@ -5439,15 +6949,25 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Tackle (psychic, 40)</t>
+          <t>Tackle (normal, 40)</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>Quick Attack (psychic, 50)</t>
+          <t>Psychic Move (psychic, 60)</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
+        <is>
+          <t>Quick Attack (normal, 50)</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Psychic Blast (psychic, 80)</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
         <is>
           <t>https://raw.githubusercontent.com/PokeAPI/sprites/master/sprites/pokemon/151.png</t>
         </is>

</xml_diff>